<commit_message>
add an intermediate option
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E2" t="n">
         <v>93</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E3" t="n">
         <v>93</v>
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E4" t="n">
         <v>93</v>
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E5" t="n">
         <v>93</v>
@@ -576,7 +576,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E6" t="n">
         <v>93</v>
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E7" t="n">
         <v>93</v>
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E8" t="n">
         <v>93</v>
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E9" t="n">
         <v>93</v>
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E10" t="n">
         <v>93</v>
@@ -696,7 +696,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E11" t="n">
         <v>93</v>
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E12" t="n">
         <v>93</v>
@@ -744,7 +744,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E13" t="n">
         <v>93</v>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E14" t="n">
         <v>93</v>
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E15" t="n">
         <v>93</v>
@@ -816,7 +816,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E16" t="n">
         <v>93</v>
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E17" t="n">
         <v>93</v>
@@ -864,7 +864,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E18" t="n">
         <v>93</v>
@@ -888,7 +888,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E19" t="n">
         <v>93</v>
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E20" t="n">
         <v>93</v>
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E21" t="n">
         <v>93</v>
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E22" t="n">
         <v>93</v>
@@ -984,7 +984,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E23" t="n">
         <v>93</v>
@@ -1008,7 +1008,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E24" t="n">
         <v>93</v>
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E25" t="n">
         <v>93</v>
@@ -1056,7 +1056,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E26" t="n">
         <v>93</v>
@@ -1080,7 +1080,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E27" t="n">
         <v>93</v>
@@ -1104,7 +1104,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E28" t="n">
         <v>93</v>
@@ -1128,7 +1128,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E29" t="n">
         <v>93</v>
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E30" t="n">
         <v>93</v>
@@ -1176,7 +1176,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E31" t="n">
         <v>93</v>
@@ -1200,7 +1200,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E32" t="n">
         <v>93</v>
@@ -1224,7 +1224,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E33" t="n">
         <v>93</v>
@@ -1248,7 +1248,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E34" t="n">
         <v>93</v>
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E35" t="n">
         <v>93</v>
@@ -1296,7 +1296,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E36" t="n">
         <v>93</v>
@@ -1320,7 +1320,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E37" t="n">
         <v>93</v>
@@ -1344,7 +1344,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E38" t="n">
         <v>93</v>
@@ -1368,7 +1368,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E39" t="n">
         <v>93</v>
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E40" t="n">
         <v>93</v>
@@ -1416,7 +1416,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E41" t="n">
         <v>93</v>
@@ -1440,7 +1440,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E42" t="n">
         <v>93</v>
@@ -1464,7 +1464,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E43" t="n">
         <v>93</v>
@@ -1488,7 +1488,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E44" t="n">
         <v>93</v>
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E45" t="n">
         <v>93</v>
@@ -1536,7 +1536,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E46" t="n">
         <v>93</v>
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E47" t="n">
         <v>93</v>
@@ -1584,7 +1584,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E48" t="n">
         <v>93</v>
@@ -1608,7 +1608,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E49" t="n">
         <v>93</v>
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E50" t="n">
         <v>93</v>
@@ -1656,7 +1656,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E51" t="n">
         <v>93</v>
@@ -1680,7 +1680,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E52" t="n">
         <v>93</v>
@@ -1704,7 +1704,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E53" t="n">
         <v>93</v>
@@ -1728,7 +1728,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E54" t="n">
         <v>93</v>
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E55" t="n">
         <v>93</v>
@@ -1776,7 +1776,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E56" t="n">
         <v>93</v>
@@ -1800,7 +1800,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E57" t="n">
         <v>93</v>
@@ -1824,7 +1824,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E58" t="n">
         <v>93</v>
@@ -1848,7 +1848,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E59" t="n">
         <v>93</v>
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E60" t="n">
         <v>93</v>
@@ -1896,7 +1896,7 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E61" t="n">
         <v>93</v>
@@ -1920,7 +1920,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E62" t="n">
         <v>93</v>
@@ -1944,7 +1944,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E63" t="n">
         <v>93</v>
@@ -1968,7 +1968,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E64" t="n">
         <v>93</v>
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E65" t="n">
         <v>93</v>
@@ -2016,7 +2016,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E66" t="n">
         <v>93</v>
@@ -2040,7 +2040,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E67" t="n">
         <v>93</v>
@@ -2064,7 +2064,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E68" t="n">
         <v>93</v>
@@ -2088,7 +2088,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E69" t="n">
         <v>93</v>
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E70" t="n">
         <v>93</v>
@@ -2136,7 +2136,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E71" t="n">
         <v>93</v>
@@ -2160,7 +2160,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E72" t="n">
         <v>93</v>
@@ -2184,7 +2184,7 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E73" t="n">
         <v>93</v>
@@ -2208,7 +2208,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E74" t="n">
         <v>93</v>
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="D75" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E75" t="n">
         <v>93</v>
@@ -2256,7 +2256,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E76" t="n">
         <v>93</v>
@@ -2280,7 +2280,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E77" t="n">
         <v>93</v>
@@ -2304,7 +2304,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E78" t="n">
         <v>93</v>
@@ -2328,7 +2328,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E79" t="n">
         <v>93</v>
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E80" t="n">
         <v>93</v>
@@ -2376,7 +2376,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E81" t="n">
         <v>93</v>
@@ -2400,7 +2400,7 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E82" t="n">
         <v>93</v>
@@ -2424,7 +2424,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E83" t="n">
         <v>93</v>
@@ -2448,7 +2448,7 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E84" t="n">
         <v>93</v>
@@ -2472,7 +2472,7 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E85" t="n">
         <v>93</v>
@@ -2496,7 +2496,7 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E86" t="n">
         <v>93</v>
@@ -2520,7 +2520,7 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E87" t="n">
         <v>93</v>
@@ -2544,7 +2544,7 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E88" t="n">
         <v>93</v>
@@ -2568,7 +2568,7 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E89" t="n">
         <v>93</v>
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E90" t="n">
         <v>93</v>
@@ -2616,7 +2616,7 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E91" t="n">
         <v>93</v>
@@ -2640,7 +2640,7 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E92" t="n">
         <v>93</v>
@@ -2664,7 +2664,7 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E93" t="n">
         <v>93</v>
@@ -2688,7 +2688,7 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E94" t="n">
         <v>93</v>
@@ -2712,7 +2712,7 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E95" t="n">
         <v>93</v>
@@ -2736,7 +2736,7 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E96" t="n">
         <v>93</v>
@@ -2760,7 +2760,7 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E97" t="n">
         <v>93</v>
@@ -2784,7 +2784,7 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E98" t="n">
         <v>93</v>
@@ -2808,7 +2808,7 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E99" t="n">
         <v>93</v>
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E100" t="n">
         <v>93</v>
@@ -2856,7 +2856,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>29806.55834889133</v>
+        <v>45038.08454668387</v>
       </c>
       <c r="E101" t="n">
         <v>93</v>

</xml_diff>